<commit_message>
Finalizing results for mesophotic + Latitude work for Barcelona Conference
</commit_message>
<xml_diff>
--- a/EcoTest.xlsx
+++ b/EcoTest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atsemel\Documents\Anats\MKMRSfish10tomesophotic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84FA2E12-8AD9-4CF5-AE4A-B735BC0EB878}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16AAC31-ECDC-4A43-9085-8FD807AD03DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8364" xr2:uid="{37D4BE6E-55E4-4E4B-9803-75E5762FCE2F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="16">
   <si>
     <t>Achziv 25</t>
   </si>
@@ -54,16 +54,25 @@
     <t>Transect level</t>
   </si>
   <si>
-    <t>Group level</t>
-  </si>
-  <si>
     <t>SdotYam 10</t>
   </si>
   <si>
     <t>Achziv10</t>
   </si>
   <si>
-    <t>check data</t>
+    <t>Group hellinger trans</t>
+  </si>
+  <si>
+    <t>Group level no trans</t>
+  </si>
+  <si>
+    <t>Sample based EcoTest for differences between rarefaction curves of the different study sites. Significant differences are in bold.</t>
+  </si>
+  <si>
+    <t>Richness</t>
+  </si>
+  <si>
+    <t>Effective Diversity</t>
   </si>
 </sst>
 </file>
@@ -88,31 +97,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="177"/>
-      <scheme val="minor"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -124,11 +127,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -137,16 +139,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -459,19 +468,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BE6952-83C4-402D-B129-C75A17B31DEB}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E28" sqref="A19:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -488,25 +498,25 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -514,58 +524,68 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>0.24399999999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="I4" s="1">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>0.17399999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="F5" s="1">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="I5" s="1">
         <v>0.03</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>0.03</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E6" s="5"/>
+      <c r="I6" s="1">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="G6" s="1">
+      <c r="J6" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="H6" s="1">
+      <c r="K6" s="1">
         <v>0.05</v>
       </c>
     </row>
@@ -574,9 +594,6 @@
         <v>7</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="6" t="s">
         <v>12</v>
       </c>
     </row>
@@ -584,29 +601,29 @@
       <c r="A11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
         <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" t="s">
-        <v>11</v>
       </c>
       <c r="K11" t="s">
         <v>0</v>
@@ -616,9 +633,12 @@
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="7">
         <v>0.184</v>
       </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="H12">
         <v>0.14399999999999999</v>
       </c>
@@ -627,13 +647,16 @@
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="4">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="7">
         <v>0.47799999999999998</v>
       </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="J13" s="5">
+      <c r="J13">
         <v>0.502</v>
       </c>
     </row>
@@ -641,9 +664,12 @@
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4">
+      <c r="B14" s="5"/>
+      <c r="C14" s="7">
         <v>0.248</v>
       </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -655,8 +681,11 @@
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="4">
-        <v>0.158</v>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="7">
+        <v>0.19</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -665,6 +694,129 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="7">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="7">
+        <v>0.318</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="7">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>0.32800000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="D26">
+        <v>0.69199999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="4">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="E28" s="8">
+        <v>4.3999999999999997E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>